<commit_message>
Use singl esession for task
</commit_message>
<xml_diff>
--- a/milestone3/scripts/milestone-3-java-context.xlsx
+++ b/milestone3/scripts/milestone-3-java-context.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/payalmantri/Desktop/practice/CS598/CS598-ML4SE-ChatGPT-analysis/milestone3/scripts/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66283458-C98C-C640-B1A2-D6C2FE4DB7B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F6FED74-8AEC-C145-ADA0-4DD754674E12}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -961,53 +961,6 @@
   </si>
   <si>
     <t>boolean queryLineConnector(int vertex, Line line) {
-        int next = getNextVertex(vertex);
-        boolean result = false;
-        if (next != -1) {
-                if (!m_b_has_attributes) {
-                        Point2D pt = new Point2D();
-                        getXY(vertex, pt);
-                        line.setStartXY(pt);
-                        getXY(next, pt);
-                        line.setEndXY(pt);
-                } else {
-                        Point pt = new Point();
-                        queryPoint(vertex, pt);
-                        line.setStart(pt);
-                        queryPoint(next, pt);
-                        line.setEnd(pt);
-                }
-                result = true;
-        }
-        return result;
-}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">boolean queryLineConnector(int vertex, Line line) {
-    int next = getNextVertex(vertex);
-    boolean has_attributes = m_b_has_attributes;
-    if (next != -1 &amp;&amp; has_attributes) {
-        Point pt = new Point();
-        queryPoint(vertex, pt);
-        line.setStart(pt);
-        queryPoint(next, pt);
-        line.setEnd(pt);
-        return true;
-    } else if (next != -1 &amp;&amp; !has_attributes) {
-        Point2D pt = new Point2D();
-        getXY(vertex, pt);
-        line.setStartXY(pt);
-        getXY(next, pt);
-        line.setEndXY(pt);
-        return true;
-    } else {
-        return false;
-    }
-}
-</t>
-  </si>
-  <si>
-    <t>boolean queryLineConnector(int vertex, Line line) {
     int next = getNextVertex(vertex);
     if (next == -1) {
         return false;
@@ -1745,18 +1698,6 @@
       {
         if (!Geometry.isMultiPath(getGeometryType(geometry)))
           return false;
-      }
-      return false;
-    }</t>
-  </si>
-  <si>
-    <t>//    Mutation 5: Add an extra condition to the if statement:
- boolean hasPointFeatures()
-    {
-      for (int geometry = getFirstGeometry(); geometry != -1; geometry = getNextGeometry(geometry))
-      {
-        if (!Geometry.isMultiPath(getGeometryType(geometry)) &amp;&amp; true)
-          return true;
       }
       return false;
     }</t>
@@ -5446,6 +5387,78 @@
   <si>
     <t>Mutant 3</t>
   </si>
+  <si>
+    <t>/    Mutation 5: Add an extra condition to the if statement:
+ boolean hasPointFeatures()
+    {
+      for (int geometry = getFirstGeometry(); geometry != -1; geometry = getNextGeometry(geometry))
+      {
+        if (!Geometry.isMultiPath(getGeometryType(geometry)) &amp;&amp; true)
+          return true;
+      }
+      return false;
+    }</t>
+  </si>
+  <si>
+    <t>boolean queryLineConnector(int vertex, Line line) {
+    int next = getNextVertex(vertex);
+    boolean has_attributes = m_b_has_attributes;
+    if (next != -1 &amp;&amp; has_attributes) {
+        Point pt = new Point();
+        queryPoint(vertex, pt);
+        line.setStart(pt);
+        queryPoint(next, pt);
+        line.setEnd(pt);
+        return true;
+    } else if (next != -1 &amp;&amp; !has_attributes) {
+        Point2D pt = new Point2D();
+        getXY(vertex, pt);
+        line.setStartXY(pt);
+        getXY(next, pt);
+        line.setEndXY(pt);
+        return true;
+    } else {
+        return false;
+    }
+}</t>
+  </si>
+  <si>
+    <t>private static boolean checkPolygonCrossesPolyline(Polygon polygon, Polyline polyline, double tolerance,
+                                                   ProgressTracker progressTracker) {
+    // Perform an initial check to see if the polygons intersect or if one is contained within the other.
+    boolean isDisjointOrContains = isPolygonDisjointOrContains(polygon, polyline, tolerance, false);
+    if (isDisjointOrContains)
+        return false;
+    // If the initial check didn't yield a definite result, proceed with detailed intersection check.
+    boolean crossesPolyline = checkPolygonCrossesPolylineImpl(polygon, polyline, tolerance, null);
+    return crossesPolyline;
+}
+private static boolean isPolygonDisjointOrContains(Polygon polygon, Polyline polyline, double tolerance,
+                                                   boolean detailedCheck) {
+    // Perform the rasterized test to determine if the polygons are disjoint or if one contains the other.
+    int relation = performRasterizedCheck(polygon, polyline, tolerance, detailedCheck);
+    // Check the relationship and return the result accordingly.
+    if (relation == Relation.disjoint || relation == Relation.contains)
+        return true;
+    else
+        return false;
+}
+private static int performRasterizedCheck(Polygon polygon, Polyline polyline, double tolerance,
+                                          boolean detailedCheck) {
+    // Perform the actual rasterized check here and return the result.
+    // This step determines the relationship between the polygon and the polyline.
+    // The specific implementation details of the rasterized check are omitted here.
+    int relation = performRasterizedCheckImpl(polygon, polyline, tolerance, detailedCheck);
+    return relation;
+}
+private static boolean checkPolygonCrossesPolylineImpl(Polygon polygon, Polyline polyline, double tolerance,
+                                                       ProgressTracker progressTracker) {
+    // Perform the detailed implementation of checking if the polygon crosses the polyline.
+    // The specific implementation details are omitted here.
+    boolean crossesPolyline = performDetailedIntersectionCheckImpl(polygon, polyline, tolerance, null);
+    return crossesPolyline;
+}</t>
+  </si>
 </sst>
 </file>
 
@@ -5463,23 +5476,27 @@
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -5523,7 +5540,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -5536,6 +5553,12 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -5756,15 +5779,15 @@
   </sheetPr>
   <dimension ref="A1:O768"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="O1" sqref="O1"/>
+      <selection pane="bottomLeft" activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="11.33203125" customWidth="1"/>
-    <col min="2" max="2" width="51.83203125" customWidth="1"/>
+    <col min="2" max="2" width="84.83203125" customWidth="1"/>
     <col min="3" max="3" width="38.1640625" customWidth="1"/>
     <col min="14" max="14" width="12.6640625" customWidth="1"/>
   </cols>
@@ -5793,7 +5816,7 @@
         <v>6</v>
       </c>
       <c r="K1" s="5" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="L1" s="5" t="s">
         <v>7</v>
@@ -6063,115 +6086,113 @@
       <c r="A9" s="3">
         <v>8</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="B9" s="9" t="s">
         <v>70</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="C9" s="8" t="s">
+        <v>336</v>
+      </c>
+      <c r="D9" s="2"/>
+      <c r="E9" s="8" t="s">
         <v>71</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>73</v>
       </c>
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
       <c r="H9" s="2"/>
       <c r="I9" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="J9" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="K9" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="J9" s="2" t="s">
+      <c r="L9" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="K9" s="2" t="s">
+      <c r="M9" s="2" t="s">
         <v>76</v>
-      </c>
-      <c r="L9" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="M9" s="2" t="s">
-        <v>78</v>
       </c>
       <c r="N9" s="2"/>
       <c r="O9" s="2" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="10" spans="1:15" ht="22.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="3">
         <v>9</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="B10" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="D10" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="E10" s="8" t="s">
         <v>81</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>83</v>
       </c>
       <c r="F10" s="2"/>
       <c r="G10" s="2"/>
       <c r="H10" s="2"/>
       <c r="I10" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="J10" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="K10" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="J10" s="2" t="s">
+      <c r="L10" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="K10" s="2" t="s">
+      <c r="M10" s="6" t="s">
         <v>86</v>
-      </c>
-      <c r="L10" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="M10" s="2" t="s">
-        <v>88</v>
       </c>
       <c r="N10" s="2"/>
       <c r="O10" s="2" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="11" spans="1:15" ht="22.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="3">
         <v>10</v>
       </c>
-      <c r="B11" s="3" t="s">
-        <v>90</v>
+      <c r="B11" s="9" t="s">
+        <v>88</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D11" s="2"/>
       <c r="E11" s="2" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="F11" s="2"/>
       <c r="G11" s="2"/>
       <c r="H11" s="2"/>
       <c r="I11" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="J11" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="K11" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="J11" s="2" t="s">
+      <c r="L11" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="K11" s="2" t="s">
+      <c r="M11" s="6" t="s">
         <v>95</v>
-      </c>
-      <c r="L11" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="M11" s="2" t="s">
-        <v>97</v>
       </c>
       <c r="N11" s="2"/>
       <c r="O11" s="2" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="12" spans="1:15" ht="22.5" customHeight="1" x14ac:dyDescent="0.15">
@@ -6179,36 +6200,36 @@
         <v>11</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="D12" s="2"/>
       <c r="E12" s="2" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="F12" s="2"/>
       <c r="G12" s="2"/>
       <c r="H12" s="2"/>
       <c r="I12" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="J12" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="K12" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="J12" s="2" t="s">
+      <c r="L12" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="K12" s="2" t="s">
+      <c r="M12" s="6" t="s">
         <v>104</v>
-      </c>
-      <c r="L12" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="M12" s="2" t="s">
-        <v>106</v>
       </c>
       <c r="N12" s="2"/>
       <c r="O12" s="2" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="13" spans="1:15" ht="22.5" customHeight="1" x14ac:dyDescent="0.15">
@@ -6216,14 +6237,14 @@
         <v>12</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="D13" s="2"/>
       <c r="E13" s="2" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="F13" s="2"/>
       <c r="G13" s="2"/>
@@ -6241,32 +6262,32 @@
         <v>13</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="D14" s="2"/>
       <c r="E14" s="2" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="F14" s="2"/>
       <c r="G14" s="2"/>
       <c r="H14" s="2"/>
       <c r="I14" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="J14" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="K14" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="J14" s="2" t="s">
+      <c r="L14" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="K14" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="L14" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="M14" s="2" t="s">
-        <v>118</v>
+      <c r="M14" s="6" t="s">
+        <v>335</v>
       </c>
       <c r="N14" s="2"/>
       <c r="O14" s="2"/>
@@ -6276,14 +6297,14 @@
         <v>14</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="D15" s="2"/>
       <c r="E15" s="2" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="F15" s="2"/>
       <c r="G15" s="2"/>
@@ -6295,7 +6316,7 @@
       <c r="M15" s="2"/>
       <c r="N15" s="2"/>
       <c r="O15" s="2" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
     </row>
     <row r="16" spans="1:15" ht="22.5" customHeight="1" x14ac:dyDescent="0.15">
@@ -6303,14 +6324,14 @@
         <v>15</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="D16" s="2"/>
       <c r="E16" s="2" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="F16" s="2"/>
       <c r="G16" s="2"/>
@@ -6322,7 +6343,7 @@
       <c r="M16" s="2"/>
       <c r="N16" s="2"/>
       <c r="O16" s="2" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
     </row>
     <row r="17" spans="1:15" ht="22.5" customHeight="1" x14ac:dyDescent="0.15">
@@ -6330,14 +6351,14 @@
         <v>16</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="D17" s="2"/>
       <c r="E17" s="2" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="F17" s="2"/>
       <c r="G17" s="2"/>
@@ -6349,7 +6370,7 @@
       <c r="M17" s="2"/>
       <c r="N17" s="2"/>
       <c r="O17" s="2" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
     </row>
     <row r="18" spans="1:15" ht="22.5" customHeight="1" x14ac:dyDescent="0.15">
@@ -6357,13 +6378,15 @@
         <v>17</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="D18" s="2"/>
-      <c r="E18" s="2"/>
+      <c r="E18" s="8" t="s">
+        <v>337</v>
+      </c>
       <c r="F18" s="2"/>
       <c r="G18" s="2"/>
       <c r="H18" s="2"/>
@@ -6374,7 +6397,7 @@
       <c r="M18" s="2"/>
       <c r="N18" s="2"/>
       <c r="O18" s="2" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
     </row>
     <row r="19" spans="1:15" ht="22.5" customHeight="1" x14ac:dyDescent="0.15">
@@ -6382,14 +6405,14 @@
         <v>18</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="D19" s="2"/>
       <c r="E19" s="2" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="F19" s="2"/>
       <c r="G19" s="2"/>
@@ -6401,7 +6424,7 @@
       <c r="M19" s="2"/>
       <c r="N19" s="2"/>
       <c r="O19" s="2" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
     </row>
     <row r="20" spans="1:15" ht="22.5" customHeight="1" x14ac:dyDescent="0.15">
@@ -6409,14 +6432,14 @@
         <v>19</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="D20" s="2"/>
       <c r="E20" s="2" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="F20" s="2"/>
       <c r="G20" s="2"/>
@@ -6428,7 +6451,7 @@
       <c r="M20" s="2"/>
       <c r="N20" s="2"/>
       <c r="O20" s="2" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
     </row>
     <row r="21" spans="1:15" ht="22.5" customHeight="1" x14ac:dyDescent="0.15">
@@ -6436,14 +6459,14 @@
         <v>20</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="D21" s="2"/>
       <c r="E21" s="2" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="F21" s="2"/>
       <c r="G21" s="2"/>
@@ -6461,14 +6484,14 @@
         <v>21</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="D22" s="2"/>
       <c r="E22" s="2" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="F22" s="2"/>
       <c r="G22" s="2"/>
@@ -6480,7 +6503,7 @@
       <c r="M22" s="2"/>
       <c r="N22" s="2"/>
       <c r="O22" s="2" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
     </row>
     <row r="23" spans="1:15" ht="22.5" customHeight="1" x14ac:dyDescent="0.15">
@@ -6488,14 +6511,14 @@
         <v>22</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="D23" s="2"/>
       <c r="E23" s="2" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="F23" s="2"/>
       <c r="G23" s="2"/>
@@ -6507,7 +6530,7 @@
       <c r="M23" s="2"/>
       <c r="N23" s="2"/>
       <c r="O23" s="2" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
     </row>
     <row r="24" spans="1:15" ht="22.5" customHeight="1" x14ac:dyDescent="0.15">
@@ -6515,14 +6538,14 @@
         <v>23</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="D24" s="2"/>
       <c r="E24" s="2" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="F24" s="2"/>
       <c r="G24" s="2"/>
@@ -6534,7 +6557,7 @@
       <c r="M24" s="2"/>
       <c r="N24" s="2"/>
       <c r="O24" s="2" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
     </row>
     <row r="25" spans="1:15" ht="22.5" customHeight="1" x14ac:dyDescent="0.15">
@@ -6542,14 +6565,14 @@
         <v>24</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="D25" s="2"/>
       <c r="E25" s="2" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="F25" s="2"/>
       <c r="G25" s="2"/>
@@ -6561,7 +6584,7 @@
       <c r="M25" s="2"/>
       <c r="N25" s="2"/>
       <c r="O25" s="2" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
     </row>
     <row r="26" spans="1:15" ht="22.5" customHeight="1" x14ac:dyDescent="0.15">
@@ -6569,14 +6592,14 @@
         <v>25</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="D26" s="2"/>
       <c r="E26" s="2" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="F26" s="2"/>
       <c r="G26" s="2"/>
@@ -6588,7 +6611,7 @@
       <c r="M26" s="2"/>
       <c r="N26" s="2"/>
       <c r="O26" s="2" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
     </row>
     <row r="27" spans="1:15" ht="22.5" customHeight="1" x14ac:dyDescent="0.15">
@@ -6596,14 +6619,14 @@
         <v>26</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="D27" s="2"/>
       <c r="E27" s="2" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="F27" s="2"/>
       <c r="G27" s="2"/>
@@ -6615,7 +6638,7 @@
       <c r="M27" s="2"/>
       <c r="N27" s="2"/>
       <c r="O27" s="2" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
     </row>
     <row r="28" spans="1:15" ht="22.5" customHeight="1" x14ac:dyDescent="0.15">
@@ -6623,36 +6646,36 @@
         <v>27</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="D28" s="2"/>
       <c r="E28" s="2" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="F28" s="2"/>
       <c r="G28" s="2"/>
       <c r="H28" s="2"/>
       <c r="I28" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="J28" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="K28" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="L28" s="2" t="s">
         <v>172</v>
       </c>
-      <c r="J28" s="2" t="s">
+      <c r="M28" s="2" t="s">
         <v>173</v>
-      </c>
-      <c r="K28" s="2" t="s">
-        <v>174</v>
-      </c>
-      <c r="L28" s="2" t="s">
-        <v>175</v>
-      </c>
-      <c r="M28" s="2" t="s">
-        <v>176</v>
       </c>
       <c r="N28" s="2"/>
       <c r="O28" s="2" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
     </row>
     <row r="29" spans="1:15" ht="22.5" customHeight="1" x14ac:dyDescent="0.15">
@@ -6660,14 +6683,14 @@
         <v>28</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="D29" s="2"/>
       <c r="E29" s="2" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="F29" s="2"/>
       <c r="G29" s="2"/>
@@ -6679,7 +6702,7 @@
       <c r="M29" s="2"/>
       <c r="N29" s="2"/>
       <c r="O29" s="2" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
     </row>
     <row r="30" spans="1:15" ht="22.5" customHeight="1" x14ac:dyDescent="0.15">
@@ -6687,14 +6710,14 @@
         <v>29</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="D30" s="2"/>
       <c r="E30" s="2" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="F30" s="2"/>
       <c r="G30" s="2"/>
@@ -6706,7 +6729,7 @@
       <c r="M30" s="2"/>
       <c r="N30" s="2"/>
       <c r="O30" s="2" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
     </row>
     <row r="31" spans="1:15" ht="22.5" customHeight="1" x14ac:dyDescent="0.15">
@@ -6714,14 +6737,14 @@
         <v>30</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="D31" s="2"/>
       <c r="E31" s="2" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="F31" s="2"/>
       <c r="G31" s="2"/>
@@ -6733,7 +6756,7 @@
       <c r="M31" s="2"/>
       <c r="N31" s="2"/>
       <c r="O31" s="2" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
     </row>
     <row r="32" spans="1:15" ht="22.5" customHeight="1" x14ac:dyDescent="0.15">
@@ -6741,14 +6764,14 @@
         <v>31</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="D32" s="2"/>
       <c r="E32" s="2" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="F32" s="2"/>
       <c r="G32" s="2"/>
@@ -6760,7 +6783,7 @@
       <c r="M32" s="2"/>
       <c r="N32" s="2"/>
       <c r="O32" s="2" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
     </row>
     <row r="33" spans="1:15" ht="22.5" customHeight="1" x14ac:dyDescent="0.15">
@@ -6768,14 +6791,14 @@
         <v>32</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="D33" s="2"/>
       <c r="E33" s="2" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="F33" s="2"/>
       <c r="G33" s="2"/>
@@ -6787,7 +6810,7 @@
       <c r="M33" s="2"/>
       <c r="N33" s="2"/>
       <c r="O33" s="2" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
     </row>
     <row r="34" spans="1:15" ht="22.5" customHeight="1" x14ac:dyDescent="0.15">
@@ -6795,14 +6818,14 @@
         <v>33</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="D34" s="2"/>
       <c r="E34" s="2" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="F34" s="2"/>
       <c r="G34" s="2"/>
@@ -6814,7 +6837,7 @@
       <c r="M34" s="2"/>
       <c r="N34" s="2"/>
       <c r="O34" s="2" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
     </row>
     <row r="35" spans="1:15" ht="22.5" customHeight="1" x14ac:dyDescent="0.15">
@@ -6822,36 +6845,36 @@
         <v>34</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="D35" s="2"/>
       <c r="E35" s="2" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="F35" s="2"/>
       <c r="G35" s="2"/>
       <c r="H35" s="2"/>
       <c r="I35" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="J35" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="K35" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="L35" s="2" t="s">
         <v>205</v>
       </c>
-      <c r="J35" s="2" t="s">
+      <c r="M35" s="2" t="s">
         <v>206</v>
-      </c>
-      <c r="K35" s="2" t="s">
-        <v>207</v>
-      </c>
-      <c r="L35" s="2" t="s">
-        <v>208</v>
-      </c>
-      <c r="M35" s="2" t="s">
-        <v>209</v>
       </c>
       <c r="N35" s="2"/>
       <c r="O35" s="2" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
     </row>
     <row r="36" spans="1:15" ht="22.5" customHeight="1" x14ac:dyDescent="0.15">
@@ -6859,14 +6882,14 @@
         <v>35</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="D36" s="2"/>
       <c r="E36" s="2" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="F36" s="2"/>
       <c r="G36" s="2"/>
@@ -6878,7 +6901,7 @@
       <c r="M36" s="2"/>
       <c r="N36" s="2"/>
       <c r="O36" s="2" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
     </row>
     <row r="37" spans="1:15" ht="22.5" customHeight="1" x14ac:dyDescent="0.15">
@@ -6886,14 +6909,14 @@
         <v>36</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="D37" s="2"/>
       <c r="E37" s="2" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="F37" s="2"/>
       <c r="G37" s="2"/>
@@ -6905,7 +6928,7 @@
       <c r="M37" s="2"/>
       <c r="N37" s="2"/>
       <c r="O37" s="2" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
     </row>
     <row r="38" spans="1:15" ht="22.5" customHeight="1" x14ac:dyDescent="0.15">
@@ -6913,14 +6936,14 @@
         <v>37</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="D38" s="2"/>
       <c r="E38" s="2" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="F38" s="2"/>
       <c r="G38" s="2"/>
@@ -6932,7 +6955,7 @@
       <c r="M38" s="2"/>
       <c r="N38" s="2"/>
       <c r="O38" s="2" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
     </row>
     <row r="39" spans="1:15" ht="22.5" customHeight="1" x14ac:dyDescent="0.15">
@@ -6940,36 +6963,36 @@
         <v>38</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="D39" s="2"/>
       <c r="E39" s="2" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="F39" s="2"/>
       <c r="G39" s="2"/>
       <c r="H39" s="2"/>
       <c r="I39" s="2" t="s">
+        <v>223</v>
+      </c>
+      <c r="J39" s="2" t="s">
+        <v>224</v>
+      </c>
+      <c r="K39" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="L39" s="2" t="s">
         <v>226</v>
       </c>
-      <c r="J39" s="2" t="s">
+      <c r="M39" s="2" t="s">
         <v>227</v>
-      </c>
-      <c r="K39" s="2" t="s">
-        <v>228</v>
-      </c>
-      <c r="L39" s="2" t="s">
-        <v>229</v>
-      </c>
-      <c r="M39" s="2" t="s">
-        <v>230</v>
       </c>
       <c r="N39" s="2"/>
       <c r="O39" s="2" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
     </row>
     <row r="40" spans="1:15" ht="22.5" customHeight="1" x14ac:dyDescent="0.15">
@@ -6977,14 +7000,14 @@
         <v>39</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="D40" s="2"/>
       <c r="E40" s="2" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="F40" s="2"/>
       <c r="G40" s="2"/>
@@ -6996,7 +7019,7 @@
       <c r="M40" s="2"/>
       <c r="N40" s="2"/>
       <c r="O40" s="2" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
     </row>
     <row r="41" spans="1:15" ht="22.5" customHeight="1" x14ac:dyDescent="0.15">
@@ -7004,36 +7027,36 @@
         <v>40</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="D41" s="2"/>
       <c r="E41" s="2" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="F41" s="2"/>
       <c r="G41" s="2"/>
       <c r="H41" s="2"/>
       <c r="I41" s="2" t="s">
+        <v>236</v>
+      </c>
+      <c r="J41" s="2" t="s">
+        <v>237</v>
+      </c>
+      <c r="K41" s="2" t="s">
+        <v>238</v>
+      </c>
+      <c r="L41" s="2" t="s">
         <v>239</v>
       </c>
-      <c r="J41" s="2" t="s">
+      <c r="M41" s="2" t="s">
         <v>240</v>
-      </c>
-      <c r="K41" s="2" t="s">
-        <v>241</v>
-      </c>
-      <c r="L41" s="2" t="s">
-        <v>242</v>
-      </c>
-      <c r="M41" s="2" t="s">
-        <v>243</v>
       </c>
       <c r="N41" s="2"/>
       <c r="O41" s="2" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
     </row>
     <row r="42" spans="1:15" ht="22.5" customHeight="1" x14ac:dyDescent="0.15">
@@ -7041,36 +7064,36 @@
         <v>41</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="D42" s="2"/>
       <c r="E42" s="2" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="F42" s="2"/>
       <c r="G42" s="2"/>
       <c r="H42" s="2"/>
       <c r="I42" s="2" t="s">
+        <v>245</v>
+      </c>
+      <c r="J42" s="2" t="s">
+        <v>246</v>
+      </c>
+      <c r="K42" s="2" t="s">
+        <v>247</v>
+      </c>
+      <c r="L42" s="2" t="s">
         <v>248</v>
       </c>
-      <c r="J42" s="2" t="s">
+      <c r="M42" s="2" t="s">
         <v>249</v>
-      </c>
-      <c r="K42" s="2" t="s">
-        <v>250</v>
-      </c>
-      <c r="L42" s="2" t="s">
-        <v>251</v>
-      </c>
-      <c r="M42" s="2" t="s">
-        <v>252</v>
       </c>
       <c r="N42" s="2"/>
       <c r="O42" s="2" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
     </row>
     <row r="43" spans="1:15" ht="22.5" customHeight="1" x14ac:dyDescent="0.15">
@@ -7078,36 +7101,36 @@
         <v>42</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="D43" s="2"/>
       <c r="E43" s="2" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="F43" s="2"/>
       <c r="G43" s="2"/>
       <c r="H43" s="2"/>
       <c r="I43" s="2" t="s">
+        <v>254</v>
+      </c>
+      <c r="J43" s="2" t="s">
+        <v>255</v>
+      </c>
+      <c r="K43" s="2" t="s">
+        <v>256</v>
+      </c>
+      <c r="L43" s="2" t="s">
         <v>257</v>
       </c>
-      <c r="J43" s="2" t="s">
+      <c r="M43" s="2" t="s">
         <v>258</v>
-      </c>
-      <c r="K43" s="2" t="s">
-        <v>259</v>
-      </c>
-      <c r="L43" s="2" t="s">
-        <v>260</v>
-      </c>
-      <c r="M43" s="2" t="s">
-        <v>261</v>
       </c>
       <c r="N43" s="2"/>
       <c r="O43" s="2" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
     </row>
     <row r="44" spans="1:15" ht="22.5" customHeight="1" x14ac:dyDescent="0.15">
@@ -7115,36 +7138,36 @@
         <v>43</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="D44" s="2"/>
       <c r="E44" s="2" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="F44" s="2"/>
       <c r="G44" s="2"/>
       <c r="H44" s="2"/>
       <c r="I44" s="2" t="s">
+        <v>263</v>
+      </c>
+      <c r="J44" s="2" t="s">
+        <v>264</v>
+      </c>
+      <c r="K44" s="2" t="s">
+        <v>265</v>
+      </c>
+      <c r="L44" s="2" t="s">
         <v>266</v>
       </c>
-      <c r="J44" s="2" t="s">
+      <c r="M44" s="2" t="s">
         <v>267</v>
-      </c>
-      <c r="K44" s="2" t="s">
-        <v>268</v>
-      </c>
-      <c r="L44" s="2" t="s">
-        <v>269</v>
-      </c>
-      <c r="M44" s="2" t="s">
-        <v>270</v>
       </c>
       <c r="N44" s="2"/>
       <c r="O44" s="2" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
     </row>
     <row r="45" spans="1:15" ht="22.5" customHeight="1" x14ac:dyDescent="0.15">
@@ -7152,36 +7175,36 @@
         <v>44</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="D45" s="2"/>
       <c r="E45" s="2" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="F45" s="2"/>
       <c r="G45" s="2"/>
       <c r="H45" s="2"/>
       <c r="I45" s="2" t="s">
+        <v>272</v>
+      </c>
+      <c r="J45" s="2" t="s">
+        <v>273</v>
+      </c>
+      <c r="K45" s="2" t="s">
+        <v>274</v>
+      </c>
+      <c r="L45" s="2" t="s">
         <v>275</v>
       </c>
-      <c r="J45" s="2" t="s">
+      <c r="M45" s="2" t="s">
         <v>276</v>
-      </c>
-      <c r="K45" s="2" t="s">
-        <v>277</v>
-      </c>
-      <c r="L45" s="2" t="s">
-        <v>278</v>
-      </c>
-      <c r="M45" s="2" t="s">
-        <v>279</v>
       </c>
       <c r="N45" s="2"/>
       <c r="O45" s="2" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
     </row>
     <row r="46" spans="1:15" ht="22.5" customHeight="1" x14ac:dyDescent="0.15">
@@ -7189,36 +7212,36 @@
         <v>45</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="D46" s="2"/>
       <c r="E46" s="2" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="F46" s="2"/>
       <c r="G46" s="2"/>
       <c r="H46" s="2"/>
       <c r="I46" s="2" t="s">
+        <v>281</v>
+      </c>
+      <c r="J46" s="2" t="s">
+        <v>282</v>
+      </c>
+      <c r="K46" s="2" t="s">
+        <v>283</v>
+      </c>
+      <c r="L46" s="2" t="s">
         <v>284</v>
       </c>
-      <c r="J46" s="2" t="s">
+      <c r="M46" s="2" t="s">
         <v>285</v>
-      </c>
-      <c r="K46" s="2" t="s">
-        <v>286</v>
-      </c>
-      <c r="L46" s="2" t="s">
-        <v>287</v>
-      </c>
-      <c r="M46" s="2" t="s">
-        <v>288</v>
       </c>
       <c r="N46" s="2"/>
       <c r="O46" s="4" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
     </row>
     <row r="47" spans="1:15" ht="22.5" customHeight="1" x14ac:dyDescent="0.15">
@@ -7226,36 +7249,36 @@
         <v>46</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="D47" s="2"/>
       <c r="E47" s="2" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="F47" s="2"/>
       <c r="G47" s="2"/>
       <c r="H47" s="2"/>
       <c r="I47" s="2" t="s">
+        <v>289</v>
+      </c>
+      <c r="J47" s="2" t="s">
+        <v>290</v>
+      </c>
+      <c r="K47" s="2" t="s">
+        <v>291</v>
+      </c>
+      <c r="L47" s="2" t="s">
         <v>292</v>
       </c>
-      <c r="J47" s="2" t="s">
+      <c r="M47" s="2" t="s">
         <v>293</v>
-      </c>
-      <c r="K47" s="2" t="s">
-        <v>294</v>
-      </c>
-      <c r="L47" s="2" t="s">
-        <v>295</v>
-      </c>
-      <c r="M47" s="2" t="s">
-        <v>296</v>
       </c>
       <c r="N47" s="2"/>
       <c r="O47" s="2" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
     </row>
     <row r="48" spans="1:15" ht="22.5" customHeight="1" x14ac:dyDescent="0.15">
@@ -7263,36 +7286,36 @@
         <v>47</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="D48" s="2"/>
       <c r="E48" s="2" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="F48" s="2"/>
       <c r="G48" s="2"/>
       <c r="H48" s="2"/>
       <c r="I48" s="2" t="s">
+        <v>298</v>
+      </c>
+      <c r="J48" s="2" t="s">
+        <v>299</v>
+      </c>
+      <c r="K48" s="2" t="s">
+        <v>300</v>
+      </c>
+      <c r="L48" s="2" t="s">
         <v>301</v>
       </c>
-      <c r="J48" s="2" t="s">
+      <c r="M48" s="2" t="s">
         <v>302</v>
-      </c>
-      <c r="K48" s="2" t="s">
-        <v>303</v>
-      </c>
-      <c r="L48" s="2" t="s">
-        <v>304</v>
-      </c>
-      <c r="M48" s="2" t="s">
-        <v>305</v>
       </c>
       <c r="N48" s="2"/>
       <c r="O48" s="2" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
     </row>
     <row r="49" spans="1:15" ht="22.5" customHeight="1" x14ac:dyDescent="0.15">
@@ -7300,36 +7323,36 @@
         <v>48</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="D49" s="2"/>
       <c r="E49" s="2" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
       <c r="F49" s="2"/>
       <c r="G49" s="2"/>
       <c r="H49" s="2"/>
       <c r="I49" s="2" t="s">
+        <v>307</v>
+      </c>
+      <c r="J49" s="2" t="s">
+        <v>308</v>
+      </c>
+      <c r="K49" s="2" t="s">
+        <v>309</v>
+      </c>
+      <c r="L49" s="2" t="s">
         <v>310</v>
       </c>
-      <c r="J49" s="2" t="s">
+      <c r="M49" s="2" t="s">
         <v>311</v>
-      </c>
-      <c r="K49" s="2" t="s">
-        <v>312</v>
-      </c>
-      <c r="L49" s="2" t="s">
-        <v>313</v>
-      </c>
-      <c r="M49" s="2" t="s">
-        <v>314</v>
       </c>
       <c r="N49" s="2"/>
       <c r="O49" s="4" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
     </row>
     <row r="50" spans="1:15" ht="22.5" customHeight="1" x14ac:dyDescent="0.15">
@@ -7337,36 +7360,36 @@
         <v>49</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
       <c r="D50" s="2"/>
       <c r="E50" s="2" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
       <c r="F50" s="2"/>
       <c r="G50" s="2"/>
       <c r="H50" s="2"/>
       <c r="I50" s="2" t="s">
+        <v>316</v>
+      </c>
+      <c r="J50" s="2" t="s">
+        <v>317</v>
+      </c>
+      <c r="K50" s="2" t="s">
+        <v>318</v>
+      </c>
+      <c r="L50" s="2" t="s">
         <v>319</v>
       </c>
-      <c r="J50" s="2" t="s">
+      <c r="M50" s="2" t="s">
         <v>320</v>
-      </c>
-      <c r="K50" s="2" t="s">
-        <v>321</v>
-      </c>
-      <c r="L50" s="2" t="s">
-        <v>322</v>
-      </c>
-      <c r="M50" s="2" t="s">
-        <v>323</v>
       </c>
       <c r="N50" s="2"/>
       <c r="O50" s="4" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
     </row>
     <row r="51" spans="1:15" ht="22.5" customHeight="1" x14ac:dyDescent="0.15">
@@ -7374,45 +7397,45 @@
         <v>50</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
       <c r="D51" s="2"/>
       <c r="E51" s="2" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="F51" s="2"/>
       <c r="G51" s="2"/>
       <c r="H51" s="2"/>
       <c r="I51" s="2" t="s">
+        <v>325</v>
+      </c>
+      <c r="J51" s="2" t="s">
+        <v>326</v>
+      </c>
+      <c r="K51" s="2" t="s">
+        <v>327</v>
+      </c>
+      <c r="L51" s="2" t="s">
         <v>328</v>
       </c>
-      <c r="J51" s="2" t="s">
+      <c r="M51" s="2" t="s">
         <v>329</v>
-      </c>
-      <c r="K51" s="2" t="s">
-        <v>330</v>
-      </c>
-      <c r="L51" s="2" t="s">
-        <v>331</v>
-      </c>
-      <c r="M51" s="2" t="s">
-        <v>332</v>
       </c>
       <c r="N51" s="2"/>
       <c r="O51" s="2" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
     </row>
     <row r="52" spans="1:15" ht="22.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A52" s="3"/>
       <c r="B52" s="3" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
       <c r="D52" s="2"/>
       <c r="E52" s="2"/>
@@ -7426,7 +7449,7 @@
       <c r="M52" s="2"/>
       <c r="N52" s="2"/>
       <c r="O52" s="2" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
     </row>
     <row r="53" spans="1:15" ht="22.5" customHeight="1" x14ac:dyDescent="0.15">

</xml_diff>